<commit_message>
Clean About page and extra years in MPNVbT, clean About page in PDiCCpDoC
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/PDiCCpDoC/Perc Decline in Cap Cost per Doubling of Cap.xlsx
+++ b/InputData/endo-learn/PDiCCpDoC/Perc Decline in Cap Cost per Doubling of Cap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="24915" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="24915" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD22"/>
     </sheetView>
   </sheetViews>
@@ -564,7 +564,7 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>